<commit_message>
Done from all classes
</commit_message>
<xml_diff>
--- a/RegularMaintenance.xlsx
+++ b/RegularMaintenance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentksuedu-my.sharepoint.com/personal/442102776_student_ksu_edu_sa/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fc223fbb64eb760/المستندات/py_camp/UNIT-1-PROJECT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{89315DE3-E208-4550-9767-E5D2DE3C693E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC19352B-C236-4125-A4C0-C82C5F1A9186}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{89315DE3-E208-4550-9767-E5D2DE3C693E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88F21677-6BFE-481C-9ACC-729343F73BAB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E47AAA6-66E3-4DD0-9172-F0DDD9F13675}"/>
+    <workbookView xWindow="5760" yWindow="1884" windowWidth="17280" windowHeight="10356" xr2:uid="{1E47AAA6-66E3-4DD0-9172-F0DDD9F13675}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>CarKilometers</t>
-  </si>
-  <si>
     <t>10,000 KM Service: Engine Oil, Oil Filter Replacement, Engine Oil Filter.</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>20,000 KM Service: Engine Oil, Oil Filter Replacement, Engine Air Filter, Cabin Filter.</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -481,9 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD904DB5-B658-4C1D-AC40-06A8FF041494}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -494,7 +492,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -511,7 +509,7 @@
         <v>250</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -522,7 +520,7 @@
         <v>400</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -533,7 +531,7 @@
         <v>250</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -544,7 +542,7 @@
         <v>550</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -555,7 +553,7 @@
         <v>250</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -566,7 +564,7 @@
         <v>900</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -577,7 +575,7 @@
         <v>250</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -588,7 +586,7 @@
         <v>550</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -599,7 +597,7 @@
         <v>250</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -610,7 +608,7 @@
         <v>1450</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>